<commit_message>
feat: Lógica fornecedores Inserida
</commit_message>
<xml_diff>
--- a/historico_vendas.xlsx
+++ b/historico_vendas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45594.09445823423</v>
+        <v>45595.1552909422</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -488,7 +488,51 @@
         <v>60</v>
       </c>
       <c r="F2" t="n">
-        <v>120</v>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45595.1552909422</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Garrafa de Água de Aço Inox</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3456</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>60</v>
+      </c>
+      <c r="F3" t="n">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45595.1552909422</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chinelo Havaiana</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>7890</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+      <c r="F4" t="n">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Problemas solucionados, subindo entrega final
</commit_message>
<xml_diff>
--- a/historico_vendas.xlsx
+++ b/historico_vendas.xlsx
@@ -471,29 +471,29 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45595.1552909422</v>
+        <v>45602.95973272563</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Garrafa de Água de Aço Inox</t>
+          <t>Teste de Fogo</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3456</v>
+        <v>2424</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>2500</v>
       </c>
       <c r="F2" t="n">
-        <v>355</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45595.1552909422</v>
+        <v>45602.96000383458</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -504,35 +504,35 @@
         <v>3456</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>60</v>
       </c>
       <c r="F3" t="n">
-        <v>355</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45595.1552909422</v>
+        <v>45602.96056168922</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Chinelo Havaiana</t>
+          <t>Livro de Receitas Vegetarianas</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7890</v>
+        <v>2345</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>35</v>
+        <v>59.9</v>
       </c>
       <c r="F4" t="n">
-        <v>355</v>
+        <v>59.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando modificações de código e documentação
</commit_message>
<xml_diff>
--- a/historico_vendas.xlsx
+++ b/historico_vendas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,68 +471,24 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45602.95973272563</v>
+        <v>45604.79457642078</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Teste de Fogo</t>
+          <t>Camiseta Estampa Animal</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2424</v>
+        <v>1234</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2500</v>
+        <v>45</v>
       </c>
       <c r="F2" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45602.96000383458</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Garrafa de Água de Aço Inox</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>3456</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>60</v>
-      </c>
-      <c r="F3" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45602.96056168922</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Livro de Receitas Vegetarianas</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2345</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>59.9</v>
-      </c>
-      <c r="F4" t="n">
-        <v>59.9</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>